<commit_message>
more brad and steves house
</commit_message>
<xml_diff>
--- a/Documentation/Pre Pro List.xlsx
+++ b/Documentation/Pre Pro List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Animation Projects\One Moon\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\Animation Projects\One Moon\OneMoon\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700A16AD-D4FE-4D76-9576-68F3137718CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5A6EFD-100B-4A07-83E8-B8E3D5141C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4C4DA91-32FA-4644-B6C6-F6AF44C314CF}"/>
+    <workbookView xWindow="7740" yWindow="2004" windowWidth="8580" windowHeight="8964" xr2:uid="{C4C4DA91-32FA-4644-B6C6-F6AF44C314CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="441">
   <si>
     <t>One Moon</t>
   </si>
@@ -1354,6 +1354,9 @@
   </si>
   <si>
     <t>Piano (Upright)</t>
+  </si>
+  <si>
+    <t>Mug - Cat mug</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83DE907-CB4D-4446-A70B-DCC626894528}">
   <dimension ref="A1:K526"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="A485" sqref="A485:A489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1782,6 +1785,9 @@
         <v>60</v>
       </c>
       <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>320</v>
+      </c>
       <c r="K5" t="s">
         <v>3</v>
       </c>
@@ -1885,6 +1891,7 @@
       <c r="A17" t="s">
         <v>55</v>
       </c>
+      <c r="B17" s="1"/>
       <c r="K17" t="s">
         <v>13</v>
       </c>
@@ -1893,6 +1900,7 @@
       <c r="A18" t="s">
         <v>56</v>
       </c>
+      <c r="B18" s="1"/>
       <c r="K18" t="s">
         <v>14</v>
       </c>
@@ -4084,7 +4092,7 @@
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
-        <v>55</v>
+        <v>440</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.3">
@@ -4474,5 +4482,6 @@
     <mergeCell ref="A50:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>